<commit_message>
more rpg fantasy encyclopedia
</commit_message>
<xml_diff>
--- a/rpg-fantasy-encyclopedia/checklist.xlsx
+++ b/rpg-fantasy-encyclopedia/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/rpg-fantasy-encyclopedia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5523BF6A-F0A4-C046-9811-6E5160209F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8C2525-F0E3-7B4B-B438-FF88B86451E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{114A4E98-C31B-7646-A1C8-8CA157B9C02D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{114A4E98-C31B-7646-A1C8-8CA157B9C02D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>year</t>
   </si>
@@ -75,14 +75,49 @@
   </si>
   <si>
     <t>RPG Fantasy Encyclopedia Japan</t>
+  </si>
+  <si>
+    <t>sword_and_magic_museum.jpg</t>
+  </si>
+  <si>
+    <t>monster_edition.jpg</t>
+  </si>
+  <si>
+    <t>monster_edition_vol2.jpg</t>
+  </si>
+  <si>
+    <t>新説 RPG幻想事典 剣と魔法の博物誌</t>
+  </si>
+  <si>
+    <t>新説RPG幻想事典 剣と魔法の博物誌~モンスター編~</t>
+  </si>
+  <si>
+    <t>新説 RPG幻想事典 剣と魔法の博物誌 ~モンスター編2~</t>
+  </si>
+  <si>
+    <t>New RPG Fantasy Encyclopedia Sword and Magic Museum</t>
+  </si>
+  <si>
+    <t>New RPG Fantasy Encyclopedia Sword and Magic Museum: Monster Edition</t>
+  </si>
+  <si>
+    <t>New RPG Illusion Encyclopedia Sword and Magic Museum: Monster Edition 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -110,8 +145,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,37 +462,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{907C6E63-ACDE-CA40-864B-4E387F03F0DF}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="37.5" customWidth="1"/>
+    <col min="2" max="2" width="54.5" customWidth="1"/>
+    <col min="3" max="3" width="66.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -497,6 +533,66 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2006</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2008</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2009</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>